<commit_message>
end of proof of concept
</commit_message>
<xml_diff>
--- a/Src/Data_files/test.xlsx
+++ b/Src/Data_files/test.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="квартири, площі" sheetId="2" r:id="rId1"/>
-    <sheet name="результат расчета программой" sheetId="4" r:id="rId2"/>
+    <sheet name="report" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="114210"/>
 </workbook>
@@ -1268,8 +1268,9 @@
   <dimension ref="A1:AP141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R110" sqref="R110"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="K108" sqref="K108"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6325,7 +6326,7 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K108" sqref="K108"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7926,5 +7927,6 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ready to refactoring for new import
</commit_message>
<xml_diff>
--- a/Src/Data_files/test.xlsx
+++ b/Src/Data_files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="квартири, площі" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
   <si>
     <t>№ квартири</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>120х30х11</t>
+  </si>
+  <si>
+    <t>10а</t>
   </si>
 </sst>
 </file>
@@ -1283,10 +1286,10 @@
   </sheetPr>
   <dimension ref="A1:AP141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K108" sqref="K108"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1894,8 +1897,8 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="13">
-        <v>10</v>
+      <c r="A16" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="B16" s="41" t="s">
         <v>12</v>
@@ -6341,7 +6344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add rull py and tests
</commit_message>
<xml_diff>
--- a/Src/Data_files/test.xlsx
+++ b/Src/Data_files/test.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="квартири, площі" sheetId="2" r:id="rId1"/>
-    <sheet name="report" sheetId="4" r:id="rId2"/>
+    <sheet name="rules" sheetId="5" r:id="rId2"/>
+    <sheet name="report" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="136">
   <si>
     <t>№ квартири</t>
   </si>
@@ -393,6 +394,36 @@
   </si>
   <si>
     <t>10а</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>rule name</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>param lengs</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>"10b" "кв.10"</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>post_divider</t>
   </si>
 </sst>
 </file>
@@ -404,7 +435,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,6 +497,12 @@
     <font>
       <sz val="11"/>
       <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1286,10 +1323,10 @@
   </sheetPr>
   <dimension ref="A1:AP141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K108" sqref="K108"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6342,9 +6379,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
+        <v>7</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New version from old comp
</commit_message>
<xml_diff>
--- a/Src/Data_files/test.xlsx
+++ b/Src/Data_files/test.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="квартири, площі" sheetId="2" r:id="rId1"/>
-    <sheet name="report" sheetId="4" r:id="rId2"/>
+    <sheet name="rules" sheetId="5" r:id="rId2"/>
+    <sheet name="Теплоенрго" sheetId="6" r:id="rId3"/>
+    <sheet name="report" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="146">
   <si>
     <t>№ квартири</t>
   </si>
@@ -393,6 +395,66 @@
   </si>
   <si>
     <t>10а</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>rule name</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>param lengs</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>"10b" "кв.10"</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>post_divider</t>
+  </si>
+  <si>
+    <t>"2b" "кв.2b"</t>
+  </si>
+  <si>
+    <t>Особовий рахунок</t>
+  </si>
+  <si>
+    <t>Адреса</t>
+  </si>
+  <si>
+    <t>№ віртуального ліч-ка</t>
+  </si>
+  <si>
+    <t>Період</t>
+  </si>
+  <si>
+    <t>Обсяг споживання,  Гкал</t>
+  </si>
+  <si>
+    <t>Всього</t>
+  </si>
+  <si>
+    <t>colmn</t>
+  </si>
+  <si>
+    <t>source ID</t>
+  </si>
+  <si>
+    <t>"3300145735" "3300145734 вулиця Скрипника, 7 кв.2b"</t>
   </si>
 </sst>
 </file>
@@ -404,7 +466,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +531,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -800,10 +874,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1009,9 +1084,11 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный_Лист2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1286,15 +1363,15 @@
   </sheetPr>
   <dimension ref="A1:AP141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K108" sqref="K108"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="13" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" style="13" bestFit="1" customWidth="1"/>
@@ -4413,7 +4490,7 @@
     </row>
     <row r="73" spans="1:19">
       <c r="A73" s="13">
-        <v>28</v>
+        <v>3300145734</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>30</v>
@@ -6342,10 +6419,797 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>3300145734</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="91" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="91">
+        <v>1</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="91">
+        <v>1</v>
+      </c>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="91">
+        <v>2</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="91">
+        <v>2</v>
+      </c>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="91">
+        <v>3</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="91">
+        <v>3</v>
+      </c>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="91">
+        <v>4</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="91">
+        <v>4</v>
+      </c>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="91">
+        <v>5</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="91">
+        <v>5</v>
+      </c>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91">
+        <v>2.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="91">
+        <v>6</v>
+      </c>
+      <c r="B7" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="91">
+        <v>6</v>
+      </c>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="91">
+        <v>7</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="91">
+        <v>7</v>
+      </c>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="91">
+        <v>8</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="91">
+        <v>8</v>
+      </c>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="91">
+        <v>9</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="91">
+        <v>9</v>
+      </c>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="91">
+        <v>11</v>
+      </c>
+      <c r="B12" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="91">
+        <v>11</v>
+      </c>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="91">
+        <v>12</v>
+      </c>
+      <c r="B13" s="91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="91">
+        <v>12</v>
+      </c>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="91">
+        <v>13</v>
+      </c>
+      <c r="B14" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="91">
+        <v>13</v>
+      </c>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="91">
+        <v>14</v>
+      </c>
+      <c r="B15" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="91">
+        <v>14</v>
+      </c>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="91">
+        <v>15</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="91">
+        <v>15</v>
+      </c>
+      <c r="D16" s="91"/>
+      <c r="E16" s="91">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="91">
+        <v>16</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="91">
+        <v>16</v>
+      </c>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="91">
+        <v>17</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="91">
+        <v>17</v>
+      </c>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="91">
+        <v>18</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="91">
+        <v>18</v>
+      </c>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="91">
+        <v>19</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="91">
+        <v>19</v>
+      </c>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="91">
+        <v>20</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="91">
+        <v>20</v>
+      </c>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="91">
+        <v>21</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="91">
+        <v>21</v>
+      </c>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="91">
+        <v>22</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="91">
+        <v>22</v>
+      </c>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="91">
+        <v>23</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="91">
+        <v>23</v>
+      </c>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="91">
+        <v>24</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="91">
+        <v>24</v>
+      </c>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="91">
+        <v>25</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="91">
+        <v>25</v>
+      </c>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="91">
+        <v>26</v>
+      </c>
+      <c r="B27" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="91">
+        <v>26</v>
+      </c>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="91">
+        <v>27</v>
+      </c>
+      <c r="B28" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="91">
+        <v>27</v>
+      </c>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13">
+        <v>3300145734</v>
+      </c>
+      <c r="B29" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="91">
+        <v>28</v>
+      </c>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="91">
+        <v>29</v>
+      </c>
+      <c r="B30" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="91">
+        <v>29</v>
+      </c>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="91">
+        <v>30</v>
+      </c>
+      <c r="B31" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="91">
+        <v>30</v>
+      </c>
+      <c r="D31" s="91"/>
+      <c r="E31" s="91">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="91">
+        <v>31</v>
+      </c>
+      <c r="B32" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="91">
+        <v>31</v>
+      </c>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="91">
+        <v>32</v>
+      </c>
+      <c r="B33" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="91">
+        <v>32</v>
+      </c>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="91">
+        <v>33</v>
+      </c>
+      <c r="B34" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="91">
+        <v>33</v>
+      </c>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="91">
+        <v>34</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="91">
+        <v>34</v>
+      </c>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="91">
+        <v>35</v>
+      </c>
+      <c r="B36" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="91">
+        <v>35</v>
+      </c>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="91">
+        <v>36</v>
+      </c>
+      <c r="B37" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="91">
+        <v>36</v>
+      </c>
+      <c r="D37" s="91"/>
+      <c r="E37" s="91">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="91">
+        <v>37</v>
+      </c>
+      <c r="B38" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="91">
+        <v>37</v>
+      </c>
+      <c r="D38" s="91"/>
+      <c r="E38" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="91">
+        <v>38</v>
+      </c>
+      <c r="B39" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="91">
+        <v>38</v>
+      </c>
+      <c r="D39" s="91"/>
+      <c r="E39" s="91">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="91"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="91"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="91" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="91">
+        <v>63.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix rules error and add test to integration_test.sh
</commit_message>
<xml_diff>
--- a/Src/Data_files/test.xlsx
+++ b/Src/Data_files/test.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="квартири, площі" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="rules" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Налаштування" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Теплоенрго" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="report" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
@@ -803,375 +803,375 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1376,78 +1376,78 @@
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="3.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="8"/>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5576,7 +5576,7 @@
       <c r="D97" s="31"/>
       <c r="E97" s="32"/>
       <c r="F97" s="32"/>
-      <c r="G97" s="0" t="n">
+      <c r="G97" s="2" t="n">
         <v>25482304</v>
       </c>
       <c r="H97" s="33" t="s">
@@ -5631,7 +5631,7 @@
       <c r="D98" s="31"/>
       <c r="E98" s="32"/>
       <c r="F98" s="32"/>
-      <c r="G98" s="0" t="n">
+      <c r="G98" s="2" t="n">
         <v>25482307</v>
       </c>
       <c r="H98" s="33" t="s">
@@ -5686,7 +5686,7 @@
       <c r="D99" s="31"/>
       <c r="E99" s="32"/>
       <c r="F99" s="32"/>
-      <c r="G99" s="0" t="n">
+      <c r="G99" s="2" t="n">
         <v>25482308</v>
       </c>
       <c r="H99" s="33" t="s">
@@ -5741,7 +5741,7 @@
       <c r="D100" s="31"/>
       <c r="E100" s="32"/>
       <c r="F100" s="32"/>
-      <c r="G100" s="0" t="n">
+      <c r="G100" s="2" t="n">
         <v>25482306</v>
       </c>
       <c r="H100" s="37" t="s">
@@ -6168,10 +6168,10 @@
       <c r="P136" s="27" t="n">
         <v>1.91808</v>
       </c>
-      <c r="R136" s="0" t="n">
+      <c r="R136" s="2" t="n">
         <v>217</v>
       </c>
-      <c r="S136" s="0" t="n">
+      <c r="S136" s="2" t="n">
         <v>146</v>
       </c>
     </row>
@@ -6224,10 +6224,10 @@
       <c r="P137" s="27" t="n">
         <v>1.91808</v>
       </c>
-      <c r="R137" s="0" t="n">
+      <c r="R137" s="2" t="n">
         <v>217</v>
       </c>
-      <c r="S137" s="0" t="n">
+      <c r="S137" s="2" t="n">
         <v>146</v>
       </c>
     </row>
@@ -6280,10 +6280,10 @@
       <c r="P138" s="27" t="n">
         <v>1.91808</v>
       </c>
-      <c r="R138" s="0" t="n">
+      <c r="R138" s="2" t="n">
         <v>217</v>
       </c>
-      <c r="S138" s="0" t="n">
+      <c r="S138" s="2" t="n">
         <v>146</v>
       </c>
     </row>
@@ -6324,10 +6324,10 @@
       <c r="P139" s="27" t="n">
         <v>1.70496</v>
       </c>
-      <c r="R139" s="0" t="n">
+      <c r="R139" s="2" t="n">
         <v>344</v>
       </c>
-      <c r="S139" s="0" t="n">
+      <c r="S139" s="2" t="n">
         <v>235</v>
       </c>
     </row>
@@ -6365,10 +6365,10 @@
       <c r="P140" s="27" t="n">
         <v>2.34432</v>
       </c>
-      <c r="R140" s="0" t="n">
+      <c r="R140" s="2" t="n">
         <v>182</v>
       </c>
-      <c r="S140" s="0" t="n">
+      <c r="S140" s="2" t="n">
         <v>120</v>
       </c>
     </row>
@@ -6406,10 +6406,10 @@
       <c r="P141" s="27" t="n">
         <v>1.70496</v>
       </c>
-      <c r="R141" s="0" t="n">
+      <c r="R141" s="2" t="n">
         <v>344</v>
       </c>
-      <c r="S141" s="0" t="n">
+      <c r="S141" s="2" t="n">
         <v>235</v>
       </c>
     </row>
@@ -6432,48 +6432,48 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -6484,30 +6484,30 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -6521,30 +6521,30 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -6558,25 +6558,25 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>3300145734</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -6604,8 +6604,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7238,8 +7238,8 @@
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="2" width="11.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="136.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>